<commit_message>
Business Case ergänzt nach Absprache mit meinem Freund Andi
</commit_message>
<xml_diff>
--- a/uebungen/Testat Business Case/Grp19_CIS_BusinessCase.xlsx
+++ b/uebungen/Testat Business Case/Grp19_CIS_BusinessCase.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="AlpineRe-BC qualitativ" sheetId="3" r:id="rId1"/>
     <sheet name="AlpineRe-BC quantitativ" sheetId="4" r:id="rId2"/>
-    <sheet name="Tabelle1" sheetId="5" r:id="rId3"/>
+    <sheet name="Fragen und Antworten" sheetId="5" r:id="rId3"/>
     <sheet name="Basis-Daten" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="115">
   <si>
     <t>Kosten
 (kCHF)</t>
@@ -357,6 +357,18 @@
   </si>
   <si>
     <t>Jahr 1 oder Jahr 0?</t>
+  </si>
+  <si>
+    <t>Rückversicherer müssen  Daten einkaufen. Reuters verkauft aktuelle Börsendaten, Firmendaten usw. Es ist wie ein Service.</t>
+  </si>
+  <si>
+    <t>Im 0ten Jahr rechnet man hoch 0 das ergibt den Faktor 1. Und im ersten Jahr wird also ohne Diskontsatz gerechnet.</t>
+  </si>
+  <si>
+    <t>Beispiel: Inflation!  Das Geld verliert an Wert und das muss man berücksichtigen. Die wichtigsten Zahlen sind der Diskontsatz und die Anzahl Jahre. Ich muss diese Zahlen runterdrücken! Ich könnte ja auch Geld in andere Projekte investieren, das muss man berücksichtigen. Der DISKONTSATZ sollte firmen-intern immer gleich sein!</t>
+  </si>
+  <si>
+    <t>Zahl ist business-abhängig und benötigt teilweise Erfahrung. Man sagt, dass das Projekt nach dem ersten Jahr noch nicht den vollen Nutzen abwirft. Denke an neue Mitarbeiter, Benutzeroberflächen welche noch nicht völlig gut bedient werden.</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1253,8 @@
   </sheetPr>
   <dimension ref="A1:XFD92"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3075,37 +3087,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="69.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3117,8 +3145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C22" sqref="A22:C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>